<commit_message>
Stand Up Andrea 25/08/20
</commit_message>
<xml_diff>
--- a/Semana 24-28 agosto/Stand_Up_Meeitng_Week_1.xlsx
+++ b/Semana 24-28 agosto/Stand_Up_Meeitng_Week_1.xlsx
@@ -5,35 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mythe\Documents\GitHub\Ingenieria_Software\Semana 24-28 agosto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paula\Documents\GitHub\Ingenieria_Software\Semana 24-28 agosto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC400CBE-931A-4325-956C-745ED0010975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268A8111-A7D7-49E1-8E49-A3CCF3D88071}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
   <si>
     <t>SEMANA 1</t>
   </si>
@@ -116,6 +108,9 @@
   </si>
   <si>
     <t>Hablar con una persona que tiene experiencia en Administracion de unidades</t>
+  </si>
+  <si>
+    <t>Leer sobre métodos, prácticas y núcleos. Pensar en clientes potenciales.</t>
   </si>
 </sst>
 </file>
@@ -433,7 +428,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -732,28 +727,28 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="7" max="7" width="22.109375" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="11" width="4.5546875" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -771,7 +766,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -787,7 +782,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -810,7 +805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
@@ -823,7 +818,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
@@ -834,7 +829,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -845,7 +840,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
@@ -862,7 +857,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
@@ -877,7 +872,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16"/>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -892,42 +887,54 @@
       <c r="F9" s="7"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="E10" s="2"/>
       <c r="F10" s="6"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="15"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="E11" s="2"/>
       <c r="F11" s="6"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="16"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="E12" s="3"/>
       <c r="F12" s="7"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>14</v>
       </c>
@@ -940,7 +947,7 @@
       <c r="F13" s="6"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
@@ -951,7 +958,7 @@
       <c r="F14" s="6"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16"/>
       <c r="B15" s="3" t="s">
         <v>10</v>
@@ -962,7 +969,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
@@ -975,7 +982,7 @@
       <c r="F16" s="6"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="15"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
@@ -986,7 +993,7 @@
       <c r="F17" s="6"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
       <c r="B18" s="4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Resumen de la tarea, que es IGLUW y daily
</commit_message>
<xml_diff>
--- a/Semana 24-28 agosto/Stand_Up_Meeitng_Week_1.xlsx
+++ b/Semana 24-28 agosto/Stand_Up_Meeitng_Week_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\57302\Documents\GitHub\Ingenieria_Software\Semana 24-28 agosto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mythe\Documents\GitHub\Ingenieria_Software\Semana 24-28 agosto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B18FE2D-D217-4566-BB88-ABE9328DB02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BE4F23-BEB3-44D5-966C-A15640251DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3320EE79-9243-42E8-8E5F-EF80DE6A9110}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="44">
   <si>
     <t>SEMANA 1</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Realizar la presentación sobre los avances obtenidos y toma de sugerencias</t>
+  </si>
+  <si>
+    <t>Se cumplio lo planeado</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -792,29 +795,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4E8726-24EF-4B21-B937-D55FA5E6EA95}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="92.6640625" customWidth="1"/>
-    <col min="4" max="4" width="206.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="121.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="92.7109375" customWidth="1"/>
+    <col min="4" max="4" width="206.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="121.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="69" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="74" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
-    <col min="10" max="10" width="10.88671875" customWidth="1"/>
-    <col min="11" max="11" width="4.5546875" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
     <col min="13" max="13" width="11" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -832,7 +835,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -848,7 +851,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -871,7 +874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
@@ -890,7 +893,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="12" t="s">
         <v>9</v>
@@ -907,7 +910,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
         <v>10</v>
@@ -924,7 +927,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
@@ -940,10 +943,14 @@
       <c r="E7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="12" t="s">
         <v>9</v>
@@ -957,10 +964,14 @@
       <c r="E8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="3" t="s">
         <v>10</v>
@@ -974,10 +985,14 @@
       <c r="E9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
@@ -1000,7 +1015,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
@@ -1021,7 +1036,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
@@ -1042,7 +1057,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>14</v>
       </c>
@@ -1065,7 +1080,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
@@ -1086,7 +1101,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="3" t="s">
         <v>10</v>
@@ -1107,7 +1122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>15</v>
       </c>
@@ -1130,7 +1145,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="12" t="s">
         <v>9</v>
@@ -1151,7 +1166,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="4" t="s">
         <v>10</v>

</xml_diff>